<commit_message>
Read TS data from excel to DataTable Process DataTable into dict Create a TimeSeries and add data to it.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,31 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\ExcelToCWMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HEC\source\repos\ExcelToCWMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCD42F8-2AE0-4844-9686-7364C1BF10CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF951EB-2E3C-4002-B612-4114D1A80E25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25095" yWindow="2955" windowWidth="17595" windowHeight="11595" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15045" yWindow="390" windowWidth="14040" windowHeight="9645" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="import" sheetId="17" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -644,7 +634,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -669,7 +659,8 @@
         <v>44256</v>
       </c>
       <c r="B2">
-        <v>121</v>
+        <f>C2</f>
+        <v>38.299999999999997</v>
       </c>
       <c r="C2">
         <v>38.299999999999997</v>
@@ -699,5 +690,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Units to Spreadsheet Added Units to TimeSeries constructor Modified ProcessDataTable to parse uot units from spreadsheet Modified input.xlsx to add units to header
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HEC\source\repos\ExcelToCWMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q0hecemt\source\repos\ExcelToCWMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF951EB-2E3C-4002-B612-4114D1A80E25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845E3A94-35D1-4D2B-B347-9D8FA92750D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15045" yWindow="390" windowWidth="14040" windowHeight="9645" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="import" sheetId="17" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,10 +35,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t>02600.Flow.Inst.~1Day.0.DailyComputed</t>
+    <t xml:space="preserve">02600.Flow.Inst.~1Day.0.DailyComputed[CFS] </t>
   </si>
   <si>
-    <t>01080.Stage.Inst.1Day.0.Manual 0700</t>
+    <t>01080.Stage.Inst.1Day.0.Manual 0700[FEET]</t>
   </si>
 </sst>
 </file>
@@ -634,16 +644,16 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.36328125" customWidth="1"/>
+    <col min="3" max="3" width="42.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44256</v>
       </c>
@@ -666,7 +676,7 @@
         <v>38.299999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44257</v>
       </c>
@@ -677,7 +687,7 @@
         <v>39.700000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44258</v>
       </c>

</xml_diff>

<commit_message>
Changed format of units input to {units=CFS}
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q0hecemt\source\repos\ExcelToCWMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845E3A94-35D1-4D2B-B347-9D8FA92750D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A9DA3C-57BD-4128-8B37-721229B11310}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,10 +35,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t xml:space="preserve">02600.Flow.Inst.~1Day.0.DailyComputed[CFS] </t>
+    <t xml:space="preserve">02600.Flow.Inst.~1Day.0.DailyComputed{units=CFS} </t>
   </si>
   <si>
-    <t>01080.Stage.Inst.1Day.0.Manual 0700[FEET]</t>
+    <t>01080.Stage.Inst.1Day.0.Manual 0700{units=FEET}</t>
   </si>
 </sst>
 </file>
@@ -649,7 +649,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.36328125" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+    <col min="2" max="2" width="43.453125" customWidth="1"/>
     <col min="3" max="3" width="42.453125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Throw an exception when {units= can not be found
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q0hecemt\source\repos\ExcelToCWMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A9DA3C-57BD-4128-8B37-721229B11310}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30339B88-7876-4463-9CF6-01918C92479B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,10 +35,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t xml:space="preserve">02600.Flow.Inst.~1Day.0.DailyComputed{units=CFS} </t>
+    <t>01080.Stage.Inst.1Day.0.Manual 0700{units=FEET}</t>
   </si>
   <si>
-    <t>01080.Stage.Inst.1Day.0.Manual 0700{units=FEET}</t>
+    <t>02600.Flow.Inst.~1Day.0.DailyComputed{units=CFS}</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,10 +659,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added ability to read timezone offset from db.config Added an offset parameter to GetTImeSeriesFromExcel Added new Excel Date parser to take care of different date formats Updated excelsheet to test against our DB
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q0hecemt\source\repos\ExcelToCWMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30339B88-7876-4463-9CF6-01918C92479B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAD1492-0FA0-4872-9DA0-D02EB7675358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="import" sheetId="17" r:id="rId1"/>
@@ -35,18 +35,19 @@
     <t>Date</t>
   </si>
   <si>
-    <t>01080.Stage.Inst.1Day.0.Manual 0700{units=FEET}</t>
+    <t>ACIA.Flow.Inst.1Hour.0.Best-NWDM{units=CFS}</t>
   </si>
   <si>
-    <t>02600.Flow.Inst.~1Day.0.DailyComputed{units=CFS}</t>
+    <t>ACIA.Stage.Inst.1Hour.0.Best-NWDM{units=FEET}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0\ ;\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="168" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -196,7 +197,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Comma0" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -641,15 +642,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAECE1B-F3C0-4870-B280-D5F084476133}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A5" sqref="A5:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.453125" customWidth="1"/>
     <col min="3" max="3" width="42.453125" customWidth="1"/>
   </cols>
@@ -659,15 +660,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44256</v>
+        <v>44348.291666666664</v>
       </c>
       <c r="B2">
         <f>C2</f>
@@ -679,7 +680,8 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44257</v>
+        <f>MROUND(A2+1, "01:00")</f>
+        <v>44349.291666666664</v>
       </c>
       <c r="B3">
         <v>121</v>
@@ -690,7 +692,8 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>44258</v>
+        <f t="shared" ref="A4:A16" si="0">MROUND(A3+1, "01:00")</f>
+        <v>44350.291666666664</v>
       </c>
       <c r="B4">
         <v>115</v>
@@ -698,6 +701,42 @@
       <c r="C4">
         <v>41.4</v>
       </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated ExcelSheet to work againts database
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q0hecemt\source\repos\ExcelToCWMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAD1492-0FA0-4872-9DA0-D02EB7675358}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4816424D-FAE4-4BBA-87FA-63A8C8C61458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -645,7 +645,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added new TimeUtilites project for handeling time zone things Updated TS.WriteToConsole to take a timezone offset so data can be displayed in the local time zone Updated Tests to indlue new timezone parameters. Removed Timezone from ParseHeader
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q0hecemt\source\repos\ExcelToCWMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4816424D-FAE4-4BBA-87FA-63A8C8C61458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F328BE-F34F-4566-B4DA-B02E70F4D900}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -645,7 +645,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,11 +671,10 @@
         <v>44348.291666666664</v>
       </c>
       <c r="B2">
-        <f>C2</f>
-        <v>38.299999999999997</v>
+        <v>100</v>
       </c>
       <c r="C2">
-        <v>38.299999999999997</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -684,10 +683,10 @@
         <v>44349.291666666664</v>
       </c>
       <c r="B3">
-        <v>121</v>
+        <v>200</v>
       </c>
       <c r="C3">
-        <v>39.700000000000003</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -696,10 +695,10 @@
         <v>44350.291666666664</v>
       </c>
       <c r="B4">
-        <v>115</v>
+        <v>300</v>
       </c>
       <c r="C4">
-        <v>41.4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Time Zone Refactoring refactored TimeSeries conversion to unix milis method Added a test demonstrating new method
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q0hecemt\source\repos\ExcelToCWMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F328BE-F34F-4566-B4DA-B02E70F4D900}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA41F838-D041-4B20-B474-5CC36038A793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12204" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="import" sheetId="17" r:id="rId1"/>
@@ -645,7 +645,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updating time zone test
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q0hecemt\source\repos\ExcelToCWMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA41F838-D041-4B20-B474-5CC36038A793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD373AB-BF25-4FF2-A724-D6A0869D6595}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12204" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="import" sheetId="17" r:id="rId1"/>
@@ -47,7 +47,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0\ ;\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="168" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -197,7 +197,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Comma0" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -645,7 +645,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44348.291666666664</v>
+        <v>44378.291666666664</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -680,7 +680,7 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>MROUND(A2+1, "01:00")</f>
-        <v>44349.291666666664</v>
+        <v>44379.291666666664</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -691,8 +691,8 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A16" si="0">MROUND(A3+1, "01:00")</f>
-        <v>44350.291666666664</v>
+        <f>MROUND(A3+1, "01:00")</f>
+        <v>44380.291666666664</v>
       </c>
       <c r="B4">
         <v>300</v>

</xml_diff>

<commit_message>
Added option to not retrive duplicate values over daylight savings threshold
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q0hecemt\source\repos\ExcelToCWMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD373AB-BF25-4FF2-A724-D6A0869D6595}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61F7F75-BE17-4395-A5A3-4F124D5605C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -642,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAECE1B-F3C0-4870-B280-D5F084476133}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44378.291666666664</v>
+        <v>44501.291666666664</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -680,7 +680,7 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>MROUND(A2+1, "01:00")</f>
-        <v>44379.291666666664</v>
+        <v>44502.291666666664</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -692,7 +692,7 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>MROUND(A3+1, "01:00")</f>
-        <v>44380.291666666664</v>
+        <v>44503.291666666664</v>
       </c>
       <c r="B4">
         <v>300</v>
@@ -702,40 +702,214 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <f>MROUND(A4+1, "01:00")</f>
+        <v>44504.291666666664</v>
+      </c>
+      <c r="B5">
+        <v>400</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <f t="shared" ref="A6:A24" si="0">MROUND(A5+1, "01:00")</f>
+        <v>44505.291666666664</v>
+      </c>
+      <c r="B6">
+        <v>500</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>44506.291666666664</v>
+      </c>
+      <c r="B7">
+        <v>600</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>44507.291666666664</v>
+      </c>
+      <c r="B8">
+        <v>700</v>
+      </c>
+      <c r="C8">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>44508.291666666664</v>
+      </c>
+      <c r="B9">
+        <v>800</v>
+      </c>
+      <c r="C9">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>44509.291666666664</v>
+      </c>
+      <c r="B10">
+        <v>900</v>
+      </c>
+      <c r="C10">
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>44510.291666666664</v>
+      </c>
+      <c r="B11">
+        <v>1000</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>44511.291666666664</v>
+      </c>
+      <c r="B12">
+        <v>1100</v>
+      </c>
+      <c r="C12">
+        <v>110</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>44512.291666666664</v>
+      </c>
+      <c r="B13">
+        <v>1200</v>
+      </c>
+      <c r="C13">
+        <v>120</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>44513.291666666664</v>
+      </c>
+      <c r="B14">
+        <v>1300</v>
+      </c>
+      <c r="C14">
+        <v>130</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>44514.291666666664</v>
+      </c>
+      <c r="B15">
+        <v>1400</v>
+      </c>
+      <c r="C15">
+        <v>140</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>44515.291666666664</v>
+      </c>
+      <c r="B16">
+        <v>1500</v>
+      </c>
+      <c r="C16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>44516.291666666664</v>
+      </c>
+      <c r="B17">
+        <v>1600</v>
+      </c>
+      <c r="C17">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>44517.291666666664</v>
+      </c>
+      <c r="B18">
+        <v>1700</v>
+      </c>
+      <c r="C18">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>44518.291666666664</v>
+      </c>
+      <c r="B19">
+        <v>1800</v>
+      </c>
+      <c r="C19">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>44519.291666666664</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>44520.291666666664</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>44521.291666666664</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>44522.291666666664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>44523.291666666664</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adjust input endTime to capture the whole day if time is not entered.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q0hecemt\source\repos\ExcelToCWMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61F7F75-BE17-4395-A5A3-4F124D5605C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F284771-24B9-4A5A-AD1E-DCF66407BF35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -645,7 +645,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,17 +886,35 @@
         <f t="shared" si="0"/>
         <v>44519.291666666664</v>
       </c>
+      <c r="B20">
+        <v>1900</v>
+      </c>
+      <c r="C20">
+        <v>190</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>44520.291666666664</v>
       </c>
+      <c r="B21">
+        <v>20000</v>
+      </c>
+      <c r="C21">
+        <v>200</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>44521.291666666664</v>
+      </c>
+      <c r="B22">
+        <v>21000</v>
+      </c>
+      <c r="C22">
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>